<commit_message>
"ONDC-DP : Added final Response changes"
</commit_message>
<xml_diff>
--- a/ondc/src/main/resources/rules/DpCalculate.xlsx
+++ b/ondc/src/main/resources/rules/DpCalculate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t xml:space="preserve">RuleSet</t>
   </si>
@@ -31,8 +31,47 @@
     <t xml:space="preserve">Import</t>
   </si>
   <si>
-    <t xml:space="preserve">com.example.ondc.model.DroolsInputDto,
-com.example.ondc.utils.DateUtils</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">com.example.ondc.model.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">DroolEngineDto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">com.example.ondc.utils.DateUtils</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -53,25 +92,7 @@
     <t xml:space="preserve">ACTION</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">$dpDto:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans Mono"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">DroolsInputDto</t>
-    </r>
+    <t xml:space="preserve">$dpDto:DroolEngineDto</t>
   </si>
   <si>
     <r>
@@ -189,35 +210,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">$</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">dpDto</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.getPincode()</t>
-    </r>
+    <t xml:space="preserve">$dpDto.getPincode()</t>
   </si>
   <si>
     <t xml:space="preserve">$1&lt;=$dpDto.getCurrentNoOfOrderInPincode() &amp;&amp; $dpDto.getCurrentNoOfOrderInPincode()&lt;=$2</t>
@@ -299,6 +292,15 @@
   </si>
   <si>
     <t xml:space="preserve">3999.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"T-Shirt"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, 10</t>
   </si>
 </sst>
 </file>
@@ -308,7 +310,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -347,21 +349,23 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="DejaVu Sans Mono"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -379,20 +383,6 @@
       <name val="DejaVu Sans Mono"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -533,7 +523,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -541,11 +531,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -557,7 +547,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -565,11 +555,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -591,12 +581,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -668,11 +658,11 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O13" activeCellId="0" sqref="O13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.57"/>
@@ -687,7 +677,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="51.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="51.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="60.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -821,7 +810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6"/>
       <c r="B7" s="12" t="s">
         <v>10</v>
@@ -981,6 +970,41 @@
       <c r="K11" s="23"/>
       <c r="L11" s="24" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="21"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="24" t="n">
+        <v>5.01</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <v>5.01</v>
+      </c>
+      <c r="N12" s="1" t="n">
+        <v>15.01</v>
+      </c>
+      <c r="O12" s="1" t="n">
+        <v>-25.01</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Added rule engine upload and download at runtime
</commit_message>
<xml_diff>
--- a/ondc/src/main/resources/rules/DpCalculate.xlsx
+++ b/ondc/src/main/resources/rules/DpCalculate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
   <si>
     <t xml:space="preserve">RuleSet</t>
   </si>
@@ -135,8 +135,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DateUtils.</t>
@@ -147,6 +147,7 @@
         <color rgb="FF000000"/>
         <rFont val="DejaVu Sans Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">isCompareDateRange</t>
     </r>
@@ -154,8 +155,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">($dpDto.getZone(),$dpDto.getZonedExpireDateTime() ,$1,$2)</t>
@@ -168,6 +169,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DateUtils.isCompareTimeRange</t>
     </r>
@@ -177,6 +179,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">( </t>
     </r>
@@ -186,6 +189,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">$dpDto.getZone(),</t>
     </r>
@@ -195,6 +199,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">$dpDto.</t>
     </r>
@@ -204,6 +209,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">getZonedExpireDateTime() ,$1,$2)</t>
     </r>
@@ -219,8 +225,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">$1&lt;=$dpDto.</t>
@@ -231,6 +237,7 @@
         <color rgb="FF000000"/>
         <rFont val="DejaVu Sans Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">getBasePrice</t>
     </r>
@@ -238,8 +245,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">() &amp;&amp; $dpDto.</t>
@@ -250,6 +257,7 @@
         <color rgb="FF000000"/>
         <rFont val="DejaVu Sans Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">getBasePrice</t>
     </r>
@@ -257,8 +265,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">()&lt;=$2</t>
@@ -284,8 +292,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">$dpDto.</t>
@@ -294,8 +302,8 @@
       <rPr>
         <sz val="13"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">setPerishablePercentage</t>
@@ -304,8 +312,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(DateUtils.isMultiple($dpDto.</t>
@@ -314,8 +322,8 @@
       <rPr>
         <sz val="13"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">getPerishableWeitage</t>
@@ -324,8 +332,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(),$param));</t>
@@ -417,6 +425,15 @@
   </si>
   <si>
     <t xml:space="preserve">30, 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Citi30"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"winter2"</t>
   </si>
 </sst>
 </file>
@@ -426,7 +443,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -494,35 +511,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans Mono"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -537,12 +529,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -625,7 +611,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -682,11 +668,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -694,10 +676,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -710,15 +688,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -736,6 +710,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -817,8 +795,8 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -983,7 +961,7 @@
       <c r="D8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="7" t="s">
@@ -998,81 +976,81 @@
       <c r="I8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="16" t="s">
+      <c r="K8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="16" t="s">
+      <c r="L8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="16" t="s">
+      <c r="M8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="N8" s="17" t="s">
+      <c r="N8" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="L9" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="M9" s="18" t="s">
+      <c r="M9" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="N9" s="18" t="s">
+      <c r="N9" s="16" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="26" t="n">
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="23" t="n">
         <v>5.01</v>
       </c>
       <c r="K10" s="1" t="n">
@@ -1086,40 +1064,40 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="21" t="s">
+      <c r="B11" s="24"/>
+      <c r="C11" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="26" t="s">
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="24" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="24"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="26" t="n">
+      <c r="H12" s="21"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="23" t="n">
         <v>5.01</v>
       </c>
       <c r="K12" s="1" t="n">
@@ -1133,24 +1111,24 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="24" t="s">
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="24"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="26" t="n">
+      <c r="H13" s="21"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="23" t="n">
         <v>-50</v>
       </c>
       <c r="K13" s="1" t="n">
@@ -1197,6 +1175,29 @@
       </c>
       <c r="N16" s="0" t="n">
         <v>-10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>